<commit_message>
Homework day09 files updated
</commit_message>
<xml_diff>
--- a/my_own_projects/theday09/atributes.xlsx
+++ b/my_own_projects/theday09/atributes.xlsx
@@ -16,10 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="55">
-  <si>
-    <t>Faktura": "Wystawiam fakturę VAT",</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="72">
   <si>
     <t>"Kolor": "inny",</t>
   </si>
@@ -181,18 +178,78 @@
   </si>
   <si>
     <t>my_file pl</t>
+  </si>
+  <si>
+    <t>"Faktura": "Wystawiam fakturę VAT",</t>
+  </si>
+  <si>
+    <t>ID oferty</t>
+  </si>
+  <si>
+    <t>ID sprzedajacego</t>
+  </si>
+  <si>
+    <t>Lokalizacja</t>
+  </si>
+  <si>
+    <t>Tytul</t>
+  </si>
+  <si>
+    <t>Cena</t>
+  </si>
+  <si>
+    <t>Marka</t>
+  </si>
+  <si>
+    <t>Model</t>
+  </si>
+  <si>
+    <t>Rok produkcji</t>
+  </si>
+  <si>
+    <t>Przebieg</t>
+  </si>
+  <si>
+    <t>Pojemność silnika</t>
+  </si>
+  <si>
+    <t>Moc</t>
+  </si>
+  <si>
+    <t>Rodzaj paliwa</t>
+  </si>
+  <si>
+    <t>Kolor</t>
+  </si>
+  <si>
+    <t>Uszkodzony</t>
+  </si>
+  <si>
+    <t>Napęd</t>
+  </si>
+  <si>
+    <t>Liczba miejsc</t>
+  </si>
+  <si>
+    <t>get offer details - key names</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Czcionka tekstu podstawowego"/>
       <family val="2"/>
+      <charset val="238"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Czcionka tekstu podstawowego"/>
       <charset val="238"/>
     </font>
   </fonts>
@@ -216,12 +273,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -518,267 +582,324 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D18"/>
+  <dimension ref="A1:F18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
     <col min="1" max="1" width="3.875" customWidth="1"/>
     <col min="2" max="2" width="16.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="35.375" style="2" customWidth="1"/>
-    <col min="4" max="4" width="30.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="35.375" style="2" customWidth="1"/>
+    <col min="5" max="5" width="2.25" style="2" customWidth="1"/>
+    <col min="6" max="6" width="30.5" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
-      <c r="B1" s="1" t="s">
+    <row r="1" spans="1:6">
+      <c r="A1" s="3"/>
+      <c r="B1" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="C1" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="D1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="F2" s="2" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
-      <c r="A2" t="s">
-        <v>51</v>
-      </c>
-      <c r="B2" t="s">
-        <v>50</v>
-      </c>
-      <c r="C2" s="2" t="s">
+    <row r="3" spans="1:6">
+      <c r="A3" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D3" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="F4" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
-      <c r="A3" t="s">
-        <v>51</v>
-      </c>
-      <c r="B3" t="s">
-        <v>17</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="D3" s="2" t="s">
+    <row r="5" spans="1:6">
+      <c r="A5" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="F5" s="2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
-      <c r="A4" t="s">
-        <v>51</v>
-      </c>
-      <c r="B4" t="s">
-        <v>18</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="D4" s="2" t="s">
+    <row r="6" spans="1:6">
+      <c r="A6" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="F7" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
-      <c r="A5" t="s">
-        <v>51</v>
-      </c>
-      <c r="B5" t="s">
-        <v>19</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4">
-      <c r="A6" t="s">
-        <v>51</v>
-      </c>
-      <c r="B6" t="s">
-        <v>20</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4">
-      <c r="A7" t="s">
-        <v>51</v>
-      </c>
-      <c r="B7" t="s">
+    <row r="8" spans="1:6">
+      <c r="A8" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="B8" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="C8" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="D8" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="F8" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
-      <c r="A8" t="s">
-        <v>51</v>
-      </c>
-      <c r="B8" t="s">
+    <row r="9" spans="1:6">
+      <c r="A9" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="B9" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="C9" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="D9" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="F9" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
-      <c r="A9" t="s">
-        <v>51</v>
-      </c>
-      <c r="B9" t="s">
+    <row r="10" spans="1:6">
+      <c r="A10" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="B10" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="C10" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="D9" s="2" t="s">
+      <c r="D10" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="F10" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
-      <c r="A10" t="s">
-        <v>51</v>
-      </c>
-      <c r="B10" t="s">
+    <row r="11" spans="1:6">
+      <c r="A11" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="B11" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="C11" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="D10" s="2" t="s">
+      <c r="D11" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="F11" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:4">
-      <c r="A11" t="s">
-        <v>51</v>
-      </c>
-      <c r="B11" t="s">
+    <row r="12" spans="1:6">
+      <c r="A12" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="B12" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="C12" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="D11" s="2" t="s">
+      <c r="D12" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="F12" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:4">
-      <c r="A12" t="s">
-        <v>51</v>
-      </c>
-      <c r="B12" t="s">
+    <row r="13" spans="1:6">
+      <c r="A13" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="B13" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="C12" s="2" t="s">
+      <c r="C13" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="D12" s="2" t="s">
+      <c r="D13" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="F13" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="13" spans="1:4">
-      <c r="A13" t="s">
-        <v>51</v>
-      </c>
-      <c r="B13" t="s">
+    <row r="14" spans="1:6">
+      <c r="A14" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="B14" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="C13" s="2" t="s">
+      <c r="C14" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="D13" s="2" t="s">
+      <c r="D14" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="F14" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="14" spans="1:4">
-      <c r="A14" t="s">
-        <v>51</v>
-      </c>
-      <c r="B14" t="s">
+    <row r="15" spans="1:6">
+      <c r="A15" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="B15" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="C14" s="2" t="s">
+      <c r="C15" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="D14" s="2" t="s">
+      <c r="D15" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="F15" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="15" spans="1:4">
-      <c r="A15" t="s">
-        <v>51</v>
-      </c>
-      <c r="B15" t="s">
+    <row r="16" spans="1:6">
+      <c r="A16" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="B16" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="C15" s="2" t="s">
+      <c r="C16" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="D15" s="2" t="s">
+      <c r="D16" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F16" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="1:4">
-      <c r="A16" t="s">
-        <v>51</v>
-      </c>
-      <c r="B16" t="s">
+    <row r="17" spans="1:6">
+      <c r="A17" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="B17" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="C16" s="2" t="s">
+      <c r="C17" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="D16" s="2" t="s">
+      <c r="D17" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="F17" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="17" spans="1:4">
-      <c r="A17" t="s">
-        <v>51</v>
-      </c>
-      <c r="B17" t="s">
+    <row r="18" spans="1:6">
+      <c r="A18" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="B18" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="C17" s="2" t="s">
+      <c r="C18" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="D17" s="2" t="s">
+      <c r="D18" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="F18" s="2" t="s">
         <v>12</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4">
-      <c r="A18" t="s">
-        <v>51</v>
-      </c>
-      <c r="B18" t="s">
-        <v>32</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>